<commit_message>
updated pom with allure reporting
</commit_message>
<xml_diff>
--- a/seleniumjava/data/TestData.xlsx
+++ b/seleniumjava/data/TestData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93C0B52-D740-43E0-9EA5-DF0474C49869}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86921CDA-3A03-45DD-A451-C37BD2E2929D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Username</t>
   </si>
@@ -364,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,14 +391,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>